<commit_message>
dev: enhance modbus byte order
</commit_message>
<xml_diff>
--- a/test/data/test-modbus-tcp-sheet.xlsx
+++ b/test/data/test-modbus-tcp-sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="28">
   <si>
     <t>tag</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>order</t>
+  </si>
+  <si>
+    <t>weight</t>
   </si>
   <si>
     <t>a1</t>
@@ -1287,10 +1290,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1305,7 +1308,7 @@
     <col min="9" max="9" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1333,13 +1336,16 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
@@ -1348,7 +1354,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -1357,18 +1363,21 @@
         <v>2</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -1377,7 +1386,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -1386,18 +1395,21 @@
         <v>2</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -1406,7 +1418,7 @@
         <v>100</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
@@ -1415,18 +1427,21 @@
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2">
         <v>3</v>
@@ -1435,7 +1450,7 @@
         <v>100</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -1444,18 +1459,21 @@
         <v>2</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2">
         <v>3</v>
@@ -1464,7 +1482,7 @@
         <v>100</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -1473,18 +1491,21 @@
         <v>2</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2">
         <v>3</v>
@@ -1493,7 +1514,7 @@
         <v>100</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
@@ -1502,18 +1523,21 @@
         <v>2</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2">
         <v>3</v>
@@ -1522,7 +1546,7 @@
         <v>100</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -1531,18 +1555,21 @@
         <v>2</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
@@ -1551,7 +1578,7 @@
         <v>100</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
@@ -1560,18 +1587,21 @@
         <v>2</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2">
         <v>3</v>
@@ -1580,7 +1610,7 @@
         <v>100</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
@@ -1589,18 +1619,21 @@
         <v>2</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2">
         <v>3</v>
@@ -1609,7 +1642,7 @@
         <v>100</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
@@ -1618,18 +1651,21 @@
         <v>2</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2">
         <v>3</v>
@@ -1638,7 +1674,7 @@
         <v>100</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F12" s="2">
         <v>0</v>
@@ -1647,18 +1683,21 @@
         <v>2</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2">
         <v>3</v>
@@ -1667,7 +1706,7 @@
         <v>100</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
@@ -1676,18 +1715,21 @@
         <v>2</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2">
         <v>3</v>
@@ -1696,7 +1738,7 @@
         <v>100</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
@@ -1705,18 +1747,21 @@
         <v>2</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2">
         <v>3</v>
@@ -1725,7 +1770,7 @@
         <v>100</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
@@ -1734,18 +1779,21 @@
         <v>2</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C16" s="2">
         <v>3</v>
@@ -1754,7 +1802,7 @@
         <v>100</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
@@ -1763,10 +1811,13 @@
         <v>2</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>